<commit_message>
creando repositorios dentro de repositorios.
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="GIT" sheetId="1" r:id="rId1"/>
+    <sheet name="Hibernate" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -73,17 +74,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,15 +102,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,13 +418,16 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="83.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -478,4 +490,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
examen git numero 2
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6EA26F-7C8E-4F51-9ADB-5BA16C71378D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GIT" sheetId="1" r:id="rId1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>git push --set-upstream origin test</t>
   </si>
@@ -145,12 +146,63 @@
   </si>
   <si>
     <t>Modifica un registro</t>
+  </si>
+  <si>
+    <t>Si al momento de querer aplicar un stash el working directory tiene cambios en los mismos archivos que dicho stash modifica:</t>
+  </si>
+  <si>
+    <t> Se aplicará pero los archivos quedarán en estado de conflicto</t>
+  </si>
+  <si>
+    <t>¿En qué se parecen un tag y un branch?</t>
+  </si>
+  <si>
+    <t>Puedo enviarlos a un repositorio remoto</t>
+  </si>
+  <si>
+    <t>Ambos apuntan a un commit </t>
+  </si>
+  <si>
+    <t>Si hago commit en el branch rama1</t>
+  </si>
+  <si>
+    <t>Solo veré el commit en el historial del branch rama1</t>
+  </si>
+  <si>
+    <t>El operador ~ indica</t>
+  </si>
+  <si>
+    <t>Previo sobre mainline</t>
+  </si>
+  <si>
+    <t>(sha)^3 funcionaría solo si</t>
+  </si>
+  <si>
+    <t>El commit tiene 3 o más parents</t>
+  </si>
+  <si>
+    <t>Un merge resuelto con estrategia fast-forward</t>
+  </si>
+  <si>
+    <t>Implica que solo una de ellas tenía contenido</t>
+  </si>
+  <si>
+    <t>Un branch o rama es:</t>
+  </si>
+  <si>
+    <t> Un puntero o variable dirigido a un commit</t>
+  </si>
+  <si>
+    <t>Si otro usuario del repositorio crea un branch:</t>
+  </si>
+  <si>
+    <t>Tendré que ejecutar git fetch para visualizar las novedades</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -206,7 +258,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -298,6 +350,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -333,6 +402,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -508,11 +594,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,6 +667,91 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -587,7 +759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -648,7 +820,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
primer examen java advance y git 3
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -3,21 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6EA26F-7C8E-4F51-9ADB-5BA16C71378D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CECCBD6E-8B93-44F0-B4EF-C889851E496E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GIT" sheetId="1" r:id="rId1"/>
     <sheet name="Hibernate" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
+    <sheet name="JAva Advance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
   <si>
     <t>git push --set-upstream origin test</t>
   </si>
@@ -197,13 +198,145 @@
   </si>
   <si>
     <t>Tendré que ejecutar git fetch para visualizar las novedades</t>
+  </si>
+  <si>
+    <t>Si revierto un cambio con git revert:</t>
+  </si>
+  <si>
+    <t>El commit original se mantendrá </t>
+  </si>
+  <si>
+    <t>Se generará un nuevo commit revirtiendo los cambios</t>
+  </si>
+  <si>
+    <t>Si utilizo git reset --hard HEAD~3 donde en HEAD hay un commit, luego una acción de merge, y luego otro commit:</t>
+  </si>
+  <si>
+    <t>Se eliminará el primer commit, la acción de merge y los commits asociados a la misma, y el tercer commit </t>
+  </si>
+  <si>
+    <t>Si modifico recursivamente el historial del repositorio (filter-branch) y hago push a un branch remoto:</t>
+  </si>
+  <si>
+    <t>El push será rechazado</t>
+  </si>
+  <si>
+    <t>Deberé realizar un push forzado</t>
+  </si>
+  <si>
+    <t>La acción de merge de otra persona descargando nuestros cambios será conflictiva</t>
+  </si>
+  <si>
+    <t>Para realizar un revert de una acción de merge necesito</t>
+  </si>
+  <si>
+    <t>Saber cual es la “mainline”</t>
+  </si>
+  <si>
+    <t>Saber cual es el commit de merge</t>
+  </si>
+  <si>
+    <t>Para reaplicar un cambio previamente revertido, puedo</t>
+  </si>
+  <si>
+    <t>Revertir el commit de revert </t>
+  </si>
+  <si>
+    <t>Volver a hacer merge del branch haciéndole un rebase para regenerar los IDs de sus commits</t>
+  </si>
+  <si>
+    <t>Para crear un thread en Java</t>
+  </si>
+  <si>
+    <t>Siempre debo extender la clase Thread.</t>
+  </si>
+  <si>
+    <t>Debo heredar de object</t>
+  </si>
+  <si>
+    <t>Puedo extender de Thread o bien implementar la interface Serializable</t>
+  </si>
+  <si>
+    <t>Ninguna es correcta</t>
+  </si>
+  <si>
+    <t>Puedo extender de Thread o bien implementar la interface Runnable</t>
+  </si>
+  <si>
+    <t>¿Que comentario es válido con respecto a la siguiente afirmación: “Un thread se “arranca” con el método start().”?</t>
+  </si>
+  <si>
+    <t>La afirmación es incorrecta</t>
+  </si>
+  <si>
+    <t>Un thread no se “arranca”, es ejecutado eventualmente por la VM. Lo único que podemos hacer como programadores es dejarlo en estado “ready” ejecutando el método “start()”.</t>
+  </si>
+  <si>
+    <t>Cuando un hilo A hace “join” sobre un hilo B…</t>
+  </si>
+  <si>
+    <t>A se frena y espera que B termine para continuar</t>
+  </si>
+  <si>
+    <t>¿Cuáles de las siguientes son ventajas del Multithreading en java?</t>
+  </si>
+  <si>
+    <t>El programador no necesita preocupar sobre si existe uno o más procesadores.</t>
+  </si>
+  <si>
+    <t>¿Cómo se llama el método donde se coloca la lógica que tendrá un hilo?</t>
+  </si>
+  <si>
+    <t>go, dc, start : ninguna es correcta</t>
+  </si>
+  <si>
+    <t>Si utilizo git cherry-pick 02kd993 y luego realizo un merge entre el branch actual y el branch origen del commit copiado:</t>
+  </si>
+  <si>
+    <t>Tendré como resultado un conflicto a resolver</t>
+  </si>
+  <si>
+    <t>Tendré dos commits con diferente SHA</t>
+  </si>
+  <si>
+    <t>Si ejecuto git rebase -i HEAD~1 invocando a la opcion “edit”:</t>
+  </si>
+  <si>
+    <t>El rebase se detiene a la espera de mi acción</t>
+  </si>
+  <si>
+    <t>git commit --amend</t>
+  </si>
+  <si>
+    <t>Añade los cambios del staging index al último commit realizado</t>
+  </si>
+  <si>
+    <t>Para dormir un hilo es necesario usar el método “sleep” de la clase Thread. ¿Cómo dormimos el hilo desde cualquier otra clase que no sea Thread?</t>
+  </si>
+  <si>
+    <t>Thread.currentThread().sleep();</t>
+  </si>
+  <si>
+    <t>Thread.sleep();</t>
+  </si>
+  <si>
+    <t>¿Que afirmación es correcta con respecto a la JVM ?</t>
+  </si>
+  <si>
+    <t>La Máquina Virtual Java (JVM) es un sistema multi-thread.</t>
+  </si>
+  <si>
+    <t>¿Cuando un hilo realiza una operación de I/O (entrada / salida) a que estado pasa?</t>
+  </si>
+  <si>
+    <t>blocked </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,6 +357,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -252,10 +391,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -596,10 +736,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,6 +890,116 @@
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -961,4 +1211,129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4188747A-658F-4585-9EFD-2B0D4552FFBF}">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>